<commit_message>
Started report and added some stats to excel
</commit_message>
<xml_diff>
--- a/Delivery 3/responses.xlsx
+++ b/Delivery 3/responses.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\HCI\Delivery 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\Documents\GitHub\HCI\Delivery 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D4F97A-BC41-4E91-8879-47ABB6A16D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171B383D-B60F-4E3A-9AD6-E20C7FA23E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5FA3DB81-35DE-4DBC-B79B-98B0620005FF}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{5FA3DB81-35DE-4DBC-B79B-98B0620005FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
   <si>
     <t>Age</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Average</t>
   </si>
   <si>
-    <t>&gt;50</t>
-  </si>
-  <si>
     <t>Std Dev</t>
   </si>
   <si>
@@ -159,6 +156,42 @@
   </si>
   <si>
     <t>average type</t>
+  </si>
+  <si>
+    <t>User characteristics</t>
+  </si>
+  <si>
+    <t>Males #</t>
+  </si>
+  <si>
+    <t>Males %</t>
+  </si>
+  <si>
+    <t>Average Age</t>
+  </si>
+  <si>
+    <t>Under 25</t>
+  </si>
+  <si>
+    <t>% under 25</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Median Age</t>
+  </si>
+  <si>
+    <t># Have used to rent</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t># Are interested</t>
+  </si>
+  <si>
+    <t>#Have rented to std</t>
   </si>
 </sst>
 </file>
@@ -295,7 +328,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -511,7 +544,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="722777824"/>
@@ -570,7 +603,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="722777408"/>
@@ -612,7 +645,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -649,7 +682,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1543,27 +1576,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1702F95B-4804-43B3-8BA4-666C96F554C6}">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.1328125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.40625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.75">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1585,8 +1621,22 @@
       <c r="H2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2">
+        <f>COUNTIF(C3:C14, "=m")</f>
+        <v>7</v>
+      </c>
+      <c r="L2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2">
+        <f>COUNTIF(F3:F14, "=1")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1611,8 +1661,22 @@
       <c r="H3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3">
+        <f>K2/COUNT(A3:A14)</f>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="L3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3">
+        <f>M2/COUNTIF(F3:F14, "&lt;&gt;")</f>
+        <v>0.22222222222222221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1637,8 +1701,22 @@
       <c r="H4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4">
+        <f>AVERAGE(B3:B14)</f>
+        <v>26.363636363636363</v>
+      </c>
+      <c r="L4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4">
+        <f>COUNTIF(H3:H14,"=1")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1663,8 +1741,22 @@
       <c r="H5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5">
+        <f>COUNTIF(B3:B14,"&lt;25")</f>
+        <v>8</v>
+      </c>
+      <c r="L5" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5">
+        <f>M4/COUNT(H3:H14,"&lt;&gt;")</f>
+        <v>0.55555555555555558</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1689,8 +1781,22 @@
       <c r="H6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6">
+        <f>K5/COUNTIF(B3:B14,"&lt;&gt;n/a")</f>
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="L6" t="s">
+        <v>51</v>
+      </c>
+      <c r="M6">
+        <f>COUNTIF(G3:G14, "=1")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1715,8 +1821,22 @@
       <c r="H7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7">
+        <f>MEDIAN(B3:B14)</f>
+        <v>20</v>
+      </c>
+      <c r="L7" t="s">
+        <v>49</v>
+      </c>
+      <c r="M7">
+        <f>M6/COUNTIF(G3:G14,"&lt;&gt;")</f>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1741,8 +1861,15 @@
       <c r="H8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8">
+        <f>COUNTIF(D3:D14, "=1")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1752,8 +1879,15 @@
       <c r="C9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>49</v>
+      </c>
+      <c r="K9">
+        <f>K8/COUNTIF(D3:D14, "&lt;&gt;")</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1778,24 +1912,41 @@
       <c r="H10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10">
+        <f>COUNTIF(E3:E14,"=1")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11">
+        <f>K10/COUNT(A3:A14)</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A12">
         <v>10</v>
       </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1821,12 +1972,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>30</v>
+      <c r="B14">
+        <v>50</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
@@ -1847,7 +1998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -1858,7 +2009,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.75">
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -1887,7 +2038,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1925,7 +2076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1963,7 +2114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2001,7 +2152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A21">
         <v>4</v>
       </c>
@@ -2039,7 +2190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A22">
         <v>5</v>
       </c>
@@ -2077,7 +2228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A23">
         <v>6</v>
       </c>
@@ -2115,7 +2266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A24">
         <v>7</v>
       </c>
@@ -2153,7 +2304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A25">
         <v>8</v>
       </c>
@@ -2191,7 +2342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A26">
         <v>9</v>
       </c>
@@ -2229,7 +2380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A27">
         <v>10</v>
       </c>
@@ -2267,7 +2418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A28">
         <v>11</v>
       </c>
@@ -2305,7 +2456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A29">
         <v>12</v>
       </c>
@@ -2343,12 +2494,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A31" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.75">
       <c r="B32" t="s">
         <v>18</v>
       </c>
@@ -2365,7 +2516,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A33">
         <v>1</v>
       </c>
@@ -2385,7 +2536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A34">
         <v>2</v>
       </c>
@@ -2405,7 +2556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2425,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2445,7 +2596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A37">
         <v>5</v>
       </c>
@@ -2465,7 +2616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A38">
         <v>6</v>
       </c>
@@ -2485,7 +2636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A39">
         <v>7</v>
       </c>
@@ -2505,7 +2656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A40">
         <v>8</v>
       </c>
@@ -2525,7 +2676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A41">
         <v>9</v>
       </c>
@@ -2545,7 +2696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A42">
         <v>10</v>
       </c>
@@ -2565,7 +2716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A43">
         <v>11</v>
       </c>
@@ -2585,7 +2736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A44">
         <v>12</v>
       </c>
@@ -2605,12 +2756,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A46" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.75">
       <c r="B47" t="s">
         <v>22</v>
       </c>
@@ -2630,7 +2781,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A48">
         <v>1</v>
       </c>
@@ -2653,7 +2804,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A49">
         <v>2</v>
       </c>
@@ -2676,7 +2827,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2699,7 +2850,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A51">
         <v>4</v>
       </c>
@@ -2722,7 +2873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A52">
         <v>5</v>
       </c>
@@ -2745,7 +2896,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A53">
         <v>6</v>
       </c>
@@ -2768,7 +2919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A54">
         <v>7</v>
       </c>
@@ -2791,7 +2942,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A55">
         <v>8</v>
       </c>
@@ -2814,7 +2965,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A56">
         <v>9</v>
       </c>
@@ -2837,7 +2988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A57">
         <v>10</v>
       </c>
@@ -2860,7 +3011,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A58">
         <v>11</v>
       </c>
@@ -2883,7 +3034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A59">
         <v>12</v>
       </c>
@@ -2906,9 +3057,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A61" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B61" t="s">
         <v>28</v>
@@ -2917,21 +3068,21 @@
         <v>29</v>
       </c>
       <c r="D61" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E61" t="s">
+        <v>35</v>
+      </c>
+      <c r="G61" t="s">
         <v>36</v>
       </c>
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>37</v>
       </c>
-      <c r="H61" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A62" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B62">
         <v>30</v>
@@ -2957,15 +3108,15 @@
         <v>47.905778453488907</v>
       </c>
       <c r="L62" t="s">
+        <v>38</v>
+      </c>
+      <c r="M62" t="s">
         <v>39</v>
       </c>
-      <c r="M62" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A63" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B63">
         <v>40</v>
@@ -3001,9 +3152,9 @@
         <v>150</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A64" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B64">
         <f>300 - O63</f>

</xml_diff>

<commit_message>
Satisfaction and clicks confidence intervals
</commit_message>
<xml_diff>
--- a/Delivery 3/responses.xlsx
+++ b/Delivery 3/responses.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\Documents\GitHub\HCI\Delivery 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\HCI\Delivery 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171B383D-B60F-4E3A-9AD6-E20C7FA23E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318A4585-3B99-4464-9DF4-CE81926D1C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{5FA3DB81-35DE-4DBC-B79B-98B0620005FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5FA3DB81-35DE-4DBC-B79B-98B0620005FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
   <si>
     <t>Age</t>
   </si>
@@ -193,12 +193,27 @@
   <si>
     <t>#Have rented to std</t>
   </si>
+  <si>
+    <t>Clicks 1</t>
+  </si>
+  <si>
+    <t>Clicks 2</t>
+  </si>
+  <si>
+    <t>Clicks 3</t>
+  </si>
+  <si>
+    <t>Satisfaction</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +225,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -328,7 +349,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -361,36 +382,36 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Questions!$H$62:$H$64</c:f>
+                <c:f>Questions!$E$62:$E$64</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>47.905778453488907</c:v>
+                    <c:v>18.459111786822248</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>40.75231530674067</c:v>
+                    <c:v>11.093148640074</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>67.136479095828548</c:v>
+                    <c:v>24.132312429161882</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Questions!$G$62:$G$64</c:f>
+                <c:f>Questions!$E$62:$E$64</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>10.987554879844414</c:v>
+                    <c:v>18.459111786822248</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>18.566018026592666</c:v>
+                    <c:v>11.093148640074</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>18.871854237504781</c:v>
+                    <c:v>24.132312429161882</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -544,7 +565,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="722777824"/>
@@ -603,7 +624,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="722777408"/>
@@ -645,7 +666,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -682,7 +703,883 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>Clicks </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-PT" baseline="0"/>
+              <a:t>(</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>Confidence Intervals)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Tests</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Questions!$E$88:$E$90</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>4.1660306298870644</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.0428116396681943</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.2828339409237111</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Questions!$E$88:$E$90</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>4.1660306298870644</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.0428116396681943</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.2828339409237111</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Questions!$A$62:$A$64</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Task1 (Search)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Task2 (Filter &amp; Order)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Task3 (Create Offer)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Questions!$C$88:$C$90</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.583333333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.958333333333334</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5B63-40E9-99F8-9838CBB42898}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Expected</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Questions!$B$88:$B$90</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5B63-40E9-99F8-9838CBB42898}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="722777408"/>
+        <c:axId val="722777824"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="722777408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="722777824"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="722777824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="722777408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>Satisfaction </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-PT" baseline="0"/>
+              <a:t>(</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>Confidence Intervals)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Tests</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Questions!$E$114:$E$116</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.1722296435936358</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.5468356784829965E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>6.690989738858924E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Questions!$E$114:$E$116</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.1722296435936358</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.5468356784829965E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>6.690989738858924E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Questions!$A$62:$A$64</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Task1 (Search)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Task2 (Filter &amp; Order)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Task3 (Create Offer)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Questions!$C$114:$C$116</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.74479166666666663</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78385416666666663</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.80989583333333337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-98D7-42E6-B5D2-14FF97CDE074}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Expected</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Questions!$B$114:$B$116</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-98D7-42E6-B5D2-14FF97CDE074}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="722777408"/>
+        <c:axId val="722777824"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="722777408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="722777824"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="722777824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="722777408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -733,7 +1630,1093 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1269,6 +3252,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>185738</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1765A056-CD19-4352-8A60-A0B24B8F4A75}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B209765-44E0-4C06-ABC7-D16EC9799E08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1574,24 +3633,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1702F95B-4804-43B3-8BA4-666C96F554C6}">
-  <dimension ref="A1:O64"/>
+  <dimension ref="A1:R116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.40625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1599,7 +3660,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1636,7 +3697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1676,7 +3737,7 @@
         <v>0.22222222222222221</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1716,7 +3777,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1756,7 +3817,7 @@
         <v>0.55555555555555558</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1796,7 +3857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1836,7 +3897,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1869,7 +3930,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1887,7 +3948,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1920,7 +3981,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1935,7 +3996,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1946,7 +4007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1972,7 +4033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1998,7 +4059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -2009,7 +4070,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -2019,6 +4080,9 @@
       <c r="D17" t="s">
         <v>13</v>
       </c>
+      <c r="E17" t="s">
+        <v>55</v>
+      </c>
       <c r="G17" t="s">
         <v>11</v>
       </c>
@@ -2028,6 +4092,9 @@
       <c r="I17" t="s">
         <v>13</v>
       </c>
+      <c r="J17" t="s">
+        <v>55</v>
+      </c>
       <c r="L17" t="s">
         <v>11</v>
       </c>
@@ -2037,8 +4104,11 @@
       <c r="N17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="O17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -2051,6 +4121,10 @@
       <c r="D18">
         <v>4</v>
       </c>
+      <c r="E18">
+        <f>(0.5 * C18 + 0.3 * (1 - B18) + 0.2 * (4 - D18))/ 1.6</f>
+        <v>0</v>
+      </c>
       <c r="F18">
         <v>1</v>
       </c>
@@ -2062,6 +4136,10 @@
       </c>
       <c r="I18">
         <v>1</v>
+      </c>
+      <c r="J18">
+        <f>(0.5 * H18 + 0.3 * (1 - G18) + 0.2 * (4 - I18))/ 1.6</f>
+        <v>0.875</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -2075,8 +4153,12 @@
       <c r="N18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="O18">
+        <f>(0.5 * M18 + 0.3 * (1 - L18) + 0.2 * (4 - N18))/ 1.6</f>
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2089,6 +4171,10 @@
       <c r="D19">
         <v>1</v>
       </c>
+      <c r="E19">
+        <f t="shared" ref="E19:E29" si="0">(0.5 * C19 + 0.3 * (1 - B19) + 0.2 * (4 - D19))/ 1.6</f>
+        <v>0.875</v>
+      </c>
       <c r="F19">
         <v>2</v>
       </c>
@@ -2101,6 +4187,10 @@
       <c r="I19">
         <v>2</v>
       </c>
+      <c r="J19">
+        <f t="shared" ref="J19:J29" si="1">(0.5 * H19 + 0.3 * (1 - G19) + 0.2 * (4 - I19))/ 1.6</f>
+        <v>0.5625</v>
+      </c>
       <c r="K19">
         <v>2</v>
       </c>
@@ -2113,8 +4203,12 @@
       <c r="N19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="O19">
+        <f t="shared" ref="O19:O29" si="2">(0.5 * M19 + 0.3 * (1 - L19) + 0.2 * (4 - N19))/ 1.6</f>
+        <v>0.6875</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2127,6 +4221,10 @@
       <c r="D20">
         <v>1</v>
       </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>0.875</v>
+      </c>
       <c r="F20">
         <v>3</v>
       </c>
@@ -2139,6 +4237,10 @@
       <c r="I20">
         <v>1</v>
       </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>0.875</v>
+      </c>
       <c r="K20">
         <v>3</v>
       </c>
@@ -2151,8 +4253,12 @@
       <c r="N20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="O20">
+        <f t="shared" si="2"/>
+        <v>0.75000000000000011</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -2165,6 +4271,10 @@
       <c r="D21">
         <v>1</v>
       </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>0.875</v>
+      </c>
       <c r="F21">
         <v>4</v>
       </c>
@@ -2177,6 +4287,10 @@
       <c r="I21">
         <v>1</v>
       </c>
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>0.875</v>
+      </c>
       <c r="K21">
         <v>4</v>
       </c>
@@ -2189,8 +4303,12 @@
       <c r="N21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="O21">
+        <f t="shared" si="2"/>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5</v>
       </c>
@@ -2203,6 +4321,10 @@
       <c r="D22">
         <v>1</v>
       </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>0.875</v>
+      </c>
       <c r="F22">
         <v>5</v>
       </c>
@@ -2215,6 +4337,10 @@
       <c r="I22">
         <v>1</v>
       </c>
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>0.875</v>
+      </c>
       <c r="K22">
         <v>5</v>
       </c>
@@ -2227,8 +4353,12 @@
       <c r="N22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="O22">
+        <f t="shared" si="2"/>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6</v>
       </c>
@@ -2241,6 +4371,10 @@
       <c r="D23">
         <v>2</v>
       </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0.5625</v>
+      </c>
       <c r="F23">
         <v>6</v>
       </c>
@@ -2253,6 +4387,10 @@
       <c r="I23">
         <v>1</v>
       </c>
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>0.6875</v>
+      </c>
       <c r="K23">
         <v>6</v>
       </c>
@@ -2265,8 +4403,12 @@
       <c r="N23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="O23">
+        <f t="shared" si="2"/>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>7</v>
       </c>
@@ -2279,6 +4421,10 @@
       <c r="D24">
         <v>2</v>
       </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>0.5625</v>
+      </c>
       <c r="F24">
         <v>7</v>
       </c>
@@ -2291,6 +4437,10 @@
       <c r="I24">
         <v>1</v>
       </c>
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>0.875</v>
+      </c>
       <c r="K24">
         <v>7</v>
       </c>
@@ -2303,8 +4453,12 @@
       <c r="N24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="O24">
+        <f t="shared" si="2"/>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>8</v>
       </c>
@@ -2317,6 +4471,10 @@
       <c r="D25">
         <v>1</v>
       </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>0.6875</v>
+      </c>
       <c r="F25">
         <v>8</v>
       </c>
@@ -2329,6 +4487,10 @@
       <c r="I25">
         <v>1</v>
       </c>
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>0.875</v>
+      </c>
       <c r="K25">
         <v>8</v>
       </c>
@@ -2341,8 +4503,12 @@
       <c r="N25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="O25">
+        <f t="shared" si="2"/>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>9</v>
       </c>
@@ -2355,6 +4521,10 @@
       <c r="D26">
         <v>1</v>
       </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>0.875</v>
+      </c>
       <c r="F26">
         <v>9</v>
       </c>
@@ -2367,6 +4537,10 @@
       <c r="I26">
         <v>1</v>
       </c>
+      <c r="J26">
+        <f t="shared" si="1"/>
+        <v>0.6875</v>
+      </c>
       <c r="K26">
         <v>9</v>
       </c>
@@ -2379,8 +4553,12 @@
       <c r="N26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="O26">
+        <f t="shared" si="2"/>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>10</v>
       </c>
@@ -2393,17 +4571,25 @@
       <c r="D27">
         <v>0</v>
       </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="F27">
         <v>10</v>
       </c>
       <c r="G27">
         <v>0</v>
       </c>
-      <c r="H27" t="s">
-        <v>15</v>
+      <c r="H27">
+        <v>0.5</v>
       </c>
       <c r="I27">
         <v>1</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="1"/>
+        <v>0.71875</v>
       </c>
       <c r="K27">
         <v>10</v>
@@ -2417,8 +4603,12 @@
       <c r="N27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="O27">
+        <f t="shared" si="2"/>
+        <v>0.71875</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>11</v>
       </c>
@@ -2431,6 +4621,10 @@
       <c r="D28">
         <v>1</v>
       </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>0.875</v>
+      </c>
       <c r="F28">
         <v>11</v>
       </c>
@@ -2443,6 +4637,10 @@
       <c r="I28">
         <v>1</v>
       </c>
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>0.875</v>
+      </c>
       <c r="K28">
         <v>11</v>
       </c>
@@ -2455,8 +4653,12 @@
       <c r="N28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="O28">
+        <f t="shared" si="2"/>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>12</v>
       </c>
@@ -2469,6 +4671,10 @@
       <c r="D29">
         <v>1</v>
       </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>0.875</v>
+      </c>
       <c r="F29">
         <v>12</v>
       </c>
@@ -2481,6 +4687,10 @@
       <c r="I29">
         <v>3</v>
       </c>
+      <c r="J29">
+        <f t="shared" si="1"/>
+        <v>0.625</v>
+      </c>
       <c r="K29">
         <v>12</v>
       </c>
@@ -2493,13 +4703,17 @@
       <c r="N29">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="O29">
+        <f t="shared" si="2"/>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>18</v>
       </c>
@@ -2516,7 +4730,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -2535,8 +4749,14 @@
       <c r="F33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="P33">
+        <v>1.4</v>
+      </c>
+      <c r="R33">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
@@ -2555,8 +4775,14 @@
       <c r="F34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="P34" t="s">
+        <v>56</v>
+      </c>
+      <c r="R34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2576,7 +4802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2596,7 +4822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>5</v>
       </c>
@@ -2616,7 +4842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>6</v>
       </c>
@@ -2636,7 +4862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>7</v>
       </c>
@@ -2656,7 +4882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>8</v>
       </c>
@@ -2676,7 +4902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>9</v>
       </c>
@@ -2696,7 +4922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>10</v>
       </c>
@@ -2716,7 +4942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>11</v>
       </c>
@@ -2736,7 +4962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>12</v>
       </c>
@@ -2756,12 +4982,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>22</v>
       </c>
@@ -2780,8 +5006,17 @@
       <c r="G47" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H47" t="s">
+        <v>52</v>
+      </c>
+      <c r="I47" t="s">
+        <v>53</v>
+      </c>
+      <c r="J47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1</v>
       </c>
@@ -2803,8 +5038,20 @@
       <c r="G48">
         <v>8</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="H48">
+        <f>3+E48</f>
+        <v>12</v>
+      </c>
+      <c r="I48">
+        <f>6+F48</f>
+        <v>6</v>
+      </c>
+      <c r="J48">
+        <f>10+G48</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2</v>
       </c>
@@ -2826,8 +5073,20 @@
       <c r="G49">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="H49">
+        <f t="shared" ref="H49:H59" si="3">3+E49</f>
+        <v>6</v>
+      </c>
+      <c r="I49">
+        <f t="shared" ref="I49:I59" si="4">6+F49</f>
+        <v>7</v>
+      </c>
+      <c r="J49">
+        <f t="shared" ref="J49:J59" si="5">10+G49</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2849,8 +5108,20 @@
       <c r="G50">
         <v>12</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="H50">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>4</v>
       </c>
@@ -2872,8 +5143,20 @@
       <c r="G51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="H51">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>5</v>
       </c>
@@ -2895,8 +5178,20 @@
       <c r="G52">
         <v>6</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="H52">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>6</v>
       </c>
@@ -2918,8 +5213,20 @@
       <c r="G53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="H53">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>7</v>
       </c>
@@ -2941,8 +5248,20 @@
       <c r="G54">
         <v>7</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="H54">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="4"/>
+        <v>38.9</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>8</v>
       </c>
@@ -2964,8 +5283,20 @@
       <c r="G55">
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="H55">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>9</v>
       </c>
@@ -2987,8 +5318,20 @@
       <c r="G56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="H56">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="4"/>
+        <v>35.6</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>10</v>
       </c>
@@ -3010,8 +5353,20 @@
       <c r="G57">
         <v>4</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="H57">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>11</v>
       </c>
@@ -3033,8 +5388,20 @@
       <c r="G58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="H58">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>12</v>
       </c>
@@ -3056,8 +5423,20 @@
       <c r="G59">
         <v>3</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="H59">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>31</v>
       </c>
@@ -3080,7 +5459,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>32</v>
       </c>
@@ -3114,7 +5493,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>33</v>
       </c>
@@ -3130,15 +5509,15 @@
         <v>17.459360843415947</v>
       </c>
       <c r="E63">
-        <f t="shared" ref="E63:E64" si="0">_xlfn.CONFIDENCE.T(0.05, D63, 12)</f>
+        <f t="shared" ref="E63:E64" si="6">_xlfn.CONFIDENCE.T(0.05, D63, 12)</f>
         <v>11.093148640074</v>
       </c>
       <c r="G63">
-        <f t="shared" ref="G63:G64" si="1">C63-E63</f>
+        <f t="shared" ref="G63:G64" si="7">C63-E63</f>
         <v>18.566018026592666</v>
       </c>
       <c r="H63">
-        <f t="shared" ref="H63:H64" si="2">C63+E63</f>
+        <f t="shared" ref="H63:H64" si="8">C63+E63</f>
         <v>40.75231530674067</v>
       </c>
       <c r="L63">
@@ -3152,7 +5531,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>34</v>
       </c>
@@ -3169,19 +5548,210 @@
         <v>37.981529352695865</v>
       </c>
       <c r="E64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>24.132312429161882</v>
       </c>
       <c r="G64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>18.871854237504781</v>
       </c>
       <c r="H64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>67.136479095828548</v>
       </c>
     </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>28</v>
+      </c>
+      <c r="C87" t="s">
+        <v>29</v>
+      </c>
+      <c r="D87" t="s">
+        <v>30</v>
+      </c>
+      <c r="E87" t="s">
+        <v>35</v>
+      </c>
+      <c r="G87" t="s">
+        <v>36</v>
+      </c>
+      <c r="H87" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>3</v>
+      </c>
+      <c r="C88">
+        <f>AVERAGE(H48:H59)</f>
+        <v>6.583333333333333</v>
+      </c>
+      <c r="D88">
+        <f>_xlfn.STDEV.S(H48:H59)</f>
+        <v>6.5568608527575334</v>
+      </c>
+      <c r="E88">
+        <f>_xlfn.CONFIDENCE.T(0.05, D88, 12)</f>
+        <v>4.1660306298870644</v>
+      </c>
+      <c r="G88">
+        <f>C88-E88</f>
+        <v>2.4173027034462686</v>
+      </c>
+      <c r="H88">
+        <f>C88+E88</f>
+        <v>10.749363963220397</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>6</v>
+      </c>
+      <c r="C89">
+        <f>AVERAGE(I48:I59)</f>
+        <v>15.958333333333334</v>
+      </c>
+      <c r="D89">
+        <f>_xlfn.STDEV.S(I48:I59)</f>
+        <v>11.08458867349646</v>
+      </c>
+      <c r="E89">
+        <f t="shared" ref="E89:E90" si="9">_xlfn.CONFIDENCE.T(0.05, D89, 12)</f>
+        <v>7.0428116396681943</v>
+      </c>
+      <c r="G89">
+        <f t="shared" ref="G89:G90" si="10">C89-E89</f>
+        <v>8.9155216936651396</v>
+      </c>
+      <c r="H89">
+        <f t="shared" ref="H89:H90" si="11">C89+E89</f>
+        <v>23.00114497300153</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>10</v>
+      </c>
+      <c r="C90">
+        <f>AVERAGE(J48:J59)</f>
+        <v>14</v>
+      </c>
+      <c r="D90">
+        <f>_xlfn.STDEV.S(J48:J59)</f>
+        <v>3.5929223355217279</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="9"/>
+        <v>2.2828339409237111</v>
+      </c>
+      <c r="G90">
+        <f t="shared" si="10"/>
+        <v>11.717166059076289</v>
+      </c>
+      <c r="H90">
+        <f t="shared" si="11"/>
+        <v>16.282833940923712</v>
+      </c>
+    </row>
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>28</v>
+      </c>
+      <c r="C113" t="s">
+        <v>29</v>
+      </c>
+      <c r="D113" t="s">
+        <v>30</v>
+      </c>
+      <c r="E113" t="s">
+        <v>35</v>
+      </c>
+      <c r="G113" t="s">
+        <v>36</v>
+      </c>
+      <c r="H113" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B114">
+        <v>0.95</v>
+      </c>
+      <c r="C114">
+        <f>AVERAGE(E18:E29)</f>
+        <v>0.74479166666666663</v>
+      </c>
+      <c r="D114">
+        <f>_xlfn.STDEV.S(E18:E29)</f>
+        <v>0.27106997237658481</v>
+      </c>
+      <c r="E114">
+        <f>_xlfn.CONFIDENCE.T(0.05, D114, 12)</f>
+        <v>0.1722296435936358</v>
+      </c>
+      <c r="G114">
+        <f>C114-E114</f>
+        <v>0.57256202307303083</v>
+      </c>
+      <c r="H114">
+        <f>C114+E114</f>
+        <v>0.91702131026030242</v>
+      </c>
+    </row>
+    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>0.9</v>
+      </c>
+      <c r="C115">
+        <f>AVERAGE(J18:J29)</f>
+        <v>0.78385416666666663</v>
+      </c>
+      <c r="D115">
+        <f>_xlfn.STDEV.S(J18:J29)</f>
+        <v>0.1187786548361994</v>
+      </c>
+      <c r="E115">
+        <f t="shared" ref="E115:E116" si="12">_xlfn.CONFIDENCE.T(0.05, D115, 12)</f>
+        <v>7.5468356784829965E-2</v>
+      </c>
+      <c r="G115">
+        <f t="shared" ref="G115:G116" si="13">C115-E115</f>
+        <v>0.70838580988183664</v>
+      </c>
+      <c r="H115">
+        <f t="shared" ref="H115:H116" si="14">C115+E115</f>
+        <v>0.85932252345149662</v>
+      </c>
+    </row>
+    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B116">
+        <v>0.85</v>
+      </c>
+      <c r="C116">
+        <f>AVERAGE(O18:O29)</f>
+        <v>0.80989583333333337</v>
+      </c>
+      <c r="D116">
+        <f>_xlfn.STDEV.S(O18:O29)</f>
+        <v>0.10530860807933076</v>
+      </c>
+      <c r="E116">
+        <f t="shared" si="12"/>
+        <v>6.690989738858924E-2</v>
+      </c>
+      <c r="G116">
+        <f t="shared" si="13"/>
+        <v>0.74298593594474416</v>
+      </c>
+      <c r="H116">
+        <f t="shared" si="14"/>
+        <v>0.87680573072192258</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>